<commit_message>
Analyzing nodetype by name
</commit_message>
<xml_diff>
--- a/UI命名2.0.xlsx
+++ b/UI命名2.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20670" windowHeight="6360"/>
@@ -19,13 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>控件类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>按扭@Button</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -82,10 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>父级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>滑动条@Slider</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>l,r,t,b;0~1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>b_,f_,h_</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -115,24 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">备注： </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1、信息记录类型的对象@Size必须放置在最后一层</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PSDName.xml</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,18 +111,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>b_,h_</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>格子@Grid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>c,r;1-n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>滑动区@ScrollView</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,10 +123,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> @Size(若伸展可不写)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>子对象命名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -201,47 +159,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Students@ScrollView</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>leftBar@Scrollbar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Progress@Slider</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserModle@Dropdown</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Name@InputField</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LogList@Group</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Persons@Grid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>red</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>面板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b_,@Size（有背景可不写）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> @Size (小格子的尺寸)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -311,7 +237,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>b_, @Size（有背景可不写）</t>
+    <t>手动条@Scrollbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v,h;0-n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b_,t_,p_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b1_,b2_,b3,t1_,t2,m_</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -319,19 +257,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>手动条@Scrollbar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v,h;0-n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b_,t_,p_</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b1_,b2_,b3,t1_,t2,m_</t>
+    <t>l,r,t,b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b_,h_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v,h;1-n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按扭@Button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>父级（可自定义）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Students@ScrollView:V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leftBar@Scrollbar:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progress@Slider:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserModle@Dropdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LogList@Group:V:0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Persons@Grid:10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -846,7 +816,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -856,31 +826,29 @@
     <col min="3" max="3" width="21.875" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>23</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G1" s="23"/>
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
       <c r="J1" s="2"/>
@@ -889,17 +857,14 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="22"/>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
       <c r="E2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -908,15 +873,15 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="B3" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -925,15 +890,15 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="6" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="18" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -942,15 +907,15 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="18" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
@@ -959,19 +924,19 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -980,17 +945,17 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="6" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="18" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -999,17 +964,17 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="18" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -1018,17 +983,17 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -1037,15 +1002,15 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="18" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -1054,15 +1019,15 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="16"/>
       <c r="F11" s="18" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
@@ -1071,17 +1036,15 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="16"/>
       <c r="F12" s="18" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1107,23 +1070,23 @@
     </row>
     <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>8</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="23" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
@@ -1131,19 +1094,19 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
@@ -1152,19 +1115,19 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
@@ -1173,19 +1136,19 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
@@ -1230,7 +1193,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1252,10 +1215,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>